<commit_message>
Update 159 result files
</commit_message>
<xml_diff>
--- a/Data/159_df_metadata_merged_landcover.xlsx
+++ b/Data/159_df_metadata_merged_landcover.xlsx
@@ -532,13 +532,13 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>66.09</v>
       </c>
       <c r="O2">
         <v>0.55</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1.84</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -618,13 +618,13 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>80.16</v>
       </c>
       <c r="O3">
         <v>4.53</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>3.49</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -704,13 +704,13 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>75.78</v>
       </c>
       <c r="O4">
         <v>4.07</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>2.37</v>
       </c>
       <c r="Q4">
         <v>0</v>
@@ -790,13 +790,13 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>67.41</v>
       </c>
       <c r="O5">
         <v>5.26</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>4.68</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -876,13 +876,13 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>77.14</v>
       </c>
       <c r="O6">
         <v>2.68</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>4.72</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -962,13 +962,13 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>71.31999999999999</v>
       </c>
       <c r="O7">
         <v>6.93</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>4.95</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1048,13 +1048,13 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>65.39</v>
       </c>
       <c r="O8">
         <v>8.49</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -1134,13 +1134,13 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>64.16</v>
       </c>
       <c r="O9">
         <v>1.96</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1.56</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1220,13 +1220,13 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>86.97674418604652</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>3.023255813953488</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1306,13 +1306,13 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>68.85775862068965</v>
       </c>
       <c r="O11">
         <v>2.155172413793104</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>2.801724137931035</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1392,13 +1392,13 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>68.85775862068965</v>
       </c>
       <c r="O12">
         <v>2.155172413793104</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>2.801724137931035</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -1478,13 +1478,13 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>67.25663716814158</v>
       </c>
       <c r="O13">
         <v>0.695322376738306</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>11.28318584070796</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -1564,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>77.14079363729094</v>
       </c>
       <c r="O14">
         <v>65.05022430368274</v>
@@ -1650,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>72.77326372661993</v>
       </c>
       <c r="O15">
         <v>54.02272694889505</v>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>87.75797758128448</v>
       </c>
       <c r="O16">
         <v>81.1697936018673</v>
@@ -1822,7 +1822,7 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>91.73114554835955</v>
       </c>
       <c r="O17">
         <v>90.50881618837407</v>
@@ -1908,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>86.29784183108426</v>
       </c>
       <c r="O18">
         <v>84.64035981020712</v>
@@ -1994,13 +1994,13 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>63.1581082885243</v>
       </c>
       <c r="O19">
         <v>4.260536067712624</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>4.353196274297732</v>
       </c>
       <c r="Q19">
         <v>1.542378801638775</v>
@@ -2080,13 +2080,13 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>80.06940831724555</v>
       </c>
       <c r="O20">
         <v>2.397611119681352</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>8.669286335698697</v>
       </c>
       <c r="Q20">
         <v>0.5106837692517379</v>
@@ -2166,13 +2166,13 @@
         <v>0.220591080837085</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>78.10793098656561</v>
       </c>
       <c r="O21">
         <v>9.694266426314282</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>8.633329400178628</v>
       </c>
       <c r="Q21">
         <v>4.504558835785655</v>
@@ -2252,13 +2252,13 @@
         <v>0</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>71.57263566006682</v>
       </c>
       <c r="O22">
         <v>2.468366603694047</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>0.2338942968605873</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2340,9 +2340,6 @@
       <c r="N23">
         <v>73.5</v>
       </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
       <c r="P23">
         <v>0</v>
       </c>
@@ -2362,9 +2359,6 @@
         <v>0</v>
       </c>
       <c r="V23">
-        <v>0</v>
-      </c>
-      <c r="W23">
         <v>0</v>
       </c>
       <c r="X23">
@@ -2426,9 +2420,6 @@
       <c r="N24">
         <v>86.2</v>
       </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
       <c r="P24">
         <v>0</v>
       </c>
@@ -2448,9 +2439,6 @@
         <v>0</v>
       </c>
       <c r="V24">
-        <v>0</v>
-      </c>
-      <c r="W24">
         <v>0</v>
       </c>
       <c r="X24">
@@ -2512,9 +2500,6 @@
       <c r="N25">
         <v>78</v>
       </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
       <c r="P25">
         <v>0</v>
       </c>
@@ -2534,9 +2519,6 @@
         <v>0</v>
       </c>
       <c r="V25">
-        <v>0</v>
-      </c>
-      <c r="W25">
         <v>0</v>
       </c>
       <c r="X25">
@@ -2598,9 +2580,6 @@
       <c r="N26">
         <v>66.09999999999999</v>
       </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
       <c r="P26">
         <v>0</v>
       </c>
@@ -2620,9 +2599,6 @@
         <v>0</v>
       </c>
       <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26">
         <v>0</v>
       </c>
       <c r="X26">
@@ -2682,13 +2658,13 @@
         <v>0</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>2.945716400218148</v>
       </c>
       <c r="O27">
         <v>0.803819074240935</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>49.19518326449716</v>
       </c>
       <c r="Q27">
         <v>5.386537440635712</v>
@@ -2768,13 +2744,13 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>50.26072108762709</v>
       </c>
       <c r="O28">
         <v>33.77815969090928</v>
       </c>
       <c r="P28">
-        <v>0</v>
+        <v>26.96750672411539</v>
       </c>
       <c r="Q28">
         <v>0</v>
@@ -2854,13 +2830,13 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>0</v>
+        <v>73.37972850445986</v>
       </c>
       <c r="O29">
         <v>32.40308010718918</v>
       </c>
       <c r="P29">
-        <v>0</v>
+        <v>13.4664149626755</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -2940,13 +2916,13 @@
         <v>0</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>0.2727278322941567</v>
       </c>
       <c r="O30">
         <v>0.2727278322941567</v>
       </c>
       <c r="P30">
-        <v>0</v>
+        <v>73.29068255796669</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -3026,13 +3002,13 @@
         <v>0</v>
       </c>
       <c r="N31">
-        <v>0</v>
+        <v>64.42741282436558</v>
       </c>
       <c r="O31">
         <v>54.1436419100796</v>
       </c>
       <c r="P31">
-        <v>0</v>
+        <v>16.59425778486688</v>
       </c>
       <c r="Q31">
         <v>2.760061364229727</v>
@@ -3112,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>75.22951658747687</v>
       </c>
       <c r="O32">
         <v>66.16502621881492</v>
@@ -3198,13 +3174,13 @@
         <v>0</v>
       </c>
       <c r="N33">
-        <v>0</v>
+        <v>37.88811769866609</v>
       </c>
       <c r="O33">
         <v>24.05474528835809</v>
       </c>
       <c r="P33">
-        <v>0</v>
+        <v>33.19745020685545</v>
       </c>
       <c r="Q33">
         <v>5.071789883028254</v>
@@ -3284,13 +3260,13 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <v>0</v>
+        <v>55.3049603754964</v>
       </c>
       <c r="O34">
         <v>47.57292436084673</v>
       </c>
       <c r="P34">
-        <v>0</v>
+        <v>13.16294143479802</v>
       </c>
       <c r="Q34">
         <v>2.237184793401103</v>
@@ -3370,13 +3346,13 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <v>0</v>
+        <v>80.47898892220675</v>
       </c>
       <c r="O35">
         <v>51.43068378640364</v>
       </c>
       <c r="P35">
-        <v>0</v>
+        <v>1.531275256514616</v>
       </c>
       <c r="Q35">
         <v>0</v>
@@ -3456,13 +3432,13 @@
         <v>0</v>
       </c>
       <c r="N36">
-        <v>0</v>
+        <v>74.94295604663255</v>
       </c>
       <c r="O36">
         <v>69.22747921339192</v>
       </c>
       <c r="P36">
-        <v>0</v>
+        <v>1.522974814360596</v>
       </c>
       <c r="Q36">
         <v>0</v>
@@ -3542,13 +3518,13 @@
         <v>0</v>
       </c>
       <c r="N37">
-        <v>0</v>
+        <v>73.11865865515256</v>
       </c>
       <c r="O37">
         <v>52.44824281014889</v>
       </c>
       <c r="P37">
-        <v>0</v>
+        <v>2.905590554754512</v>
       </c>
       <c r="Q37">
         <v>0</v>
@@ -3628,13 +3604,13 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>0</v>
+        <v>74.11244287002191</v>
       </c>
       <c r="O38">
         <v>46.30612694385988</v>
       </c>
       <c r="P38">
-        <v>0</v>
+        <v>0.5811948430577305</v>
       </c>
       <c r="Q38">
         <v>0</v>
@@ -3714,13 +3690,13 @@
         <v>4.91649504211248</v>
       </c>
       <c r="N39">
-        <v>0</v>
+        <v>55.96222429175471</v>
       </c>
       <c r="O39">
         <v>1.978093763799698</v>
       </c>
       <c r="P39">
-        <v>0</v>
+        <v>10.9298737412319</v>
       </c>
       <c r="Q39">
         <v>3.73539243850056</v>
@@ -3800,13 +3776,13 @@
         <v>2.679134393080659</v>
       </c>
       <c r="N40">
-        <v>0</v>
+        <v>54.58951727302779</v>
       </c>
       <c r="O40">
         <v>9.862456853532791</v>
       </c>
       <c r="P40">
-        <v>0</v>
+        <v>2.086250970151851</v>
       </c>
       <c r="Q40">
         <v>1.257598222939876</v>
@@ -3886,13 +3862,13 @@
         <v>6.987796089961732</v>
       </c>
       <c r="N41">
-        <v>0</v>
+        <v>67.99081269047588</v>
       </c>
       <c r="O41">
         <v>9.30492768767775</v>
       </c>
       <c r="P41">
-        <v>0</v>
+        <v>4.217153810347236</v>
       </c>
       <c r="Q41">
         <v>2.087394635361917</v>
@@ -3972,13 +3948,13 @@
         <v>0.6119208058315428</v>
       </c>
       <c r="N42">
-        <v>0</v>
+        <v>71.67161998732814</v>
       </c>
       <c r="O42">
         <v>17.22272764453717</v>
       </c>
       <c r="P42">
-        <v>0</v>
+        <v>7.036012078981011</v>
       </c>
       <c r="Q42">
         <v>4.236464890925911</v>
@@ -4058,7 +4034,7 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <v>0</v>
+        <v>62.19209565382619</v>
       </c>
       <c r="O43">
         <v>5.980637040399652</v>
@@ -4144,13 +4120,13 @@
         <v>18.49625872954079</v>
       </c>
       <c r="N44">
-        <v>0</v>
+        <v>56.97349128653126</v>
       </c>
       <c r="O44">
         <v>5.7139071956448</v>
       </c>
       <c r="P44">
-        <v>0</v>
+        <v>9.838022783602561</v>
       </c>
       <c r="Q44">
         <v>5.344393555717073</v>
@@ -4230,13 +4206,13 @@
         <v>0.7125563579458127</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>62.7962522322463</v>
       </c>
       <c r="O45">
         <v>10.96615870956933</v>
       </c>
       <c r="P45">
-        <v>0</v>
+        <v>4.795516923097312</v>
       </c>
       <c r="Q45">
         <v>4.330321314936567</v>
@@ -4316,13 +4292,13 @@
         <v>0</v>
       </c>
       <c r="N46">
-        <v>0</v>
+        <v>81.42929255682996</v>
       </c>
       <c r="O46">
         <v>26.02474585362097</v>
       </c>
       <c r="P46">
-        <v>0</v>
+        <v>6.042605533863371</v>
       </c>
       <c r="Q46">
         <v>2.357011920641038</v>
@@ -4402,13 +4378,13 @@
         <v>0</v>
       </c>
       <c r="N47">
-        <v>0</v>
+        <v>64.1999107390167</v>
       </c>
       <c r="O47">
         <v>1.555385211782272</v>
       </c>
       <c r="P47">
-        <v>0</v>
+        <v>8.53802921484565</v>
       </c>
       <c r="Q47">
         <v>1.484086733879446</v>
@@ -4488,13 +4464,13 @@
         <v>1.428651287822474</v>
       </c>
       <c r="N48">
-        <v>0</v>
+        <v>52.50143251260668</v>
       </c>
       <c r="O48">
         <v>9.274604012380257</v>
       </c>
       <c r="P48">
-        <v>0</v>
+        <v>2.170323957585325</v>
       </c>
       <c r="Q48">
         <v>1.265115344639808</v>
@@ -4574,13 +4550,13 @@
         <v>0</v>
       </c>
       <c r="N49">
-        <v>0</v>
+        <v>64.12528125592797</v>
       </c>
       <c r="O49">
         <v>0.742293237546232</v>
       </c>
       <c r="P49">
-        <v>0</v>
+        <v>2.071831132815165</v>
       </c>
       <c r="Q49">
         <v>1.668780455494413</v>
@@ -4660,13 +4636,13 @@
         <v>0</v>
       </c>
       <c r="N50">
-        <v>0</v>
+        <v>65.42007533104091</v>
       </c>
       <c r="O50">
         <v>1.430497394147251</v>
       </c>
       <c r="P50">
-        <v>0</v>
+        <v>5.777925058623288</v>
       </c>
       <c r="Q50">
         <v>1.653267059405602</v>
@@ -4746,13 +4722,13 @@
         <v>0</v>
       </c>
       <c r="N51">
-        <v>0</v>
+        <v>78.76049247193396</v>
       </c>
       <c r="O51">
         <v>2.453488545903281</v>
       </c>
       <c r="P51">
-        <v>0</v>
+        <v>6.639165919957398</v>
       </c>
       <c r="Q51">
         <v>0</v>
@@ -4832,13 +4808,13 @@
         <v>0</v>
       </c>
       <c r="N52">
-        <v>0</v>
+        <v>63.56529815952911</v>
       </c>
       <c r="O52">
         <v>11.28985193103426</v>
       </c>
       <c r="P52">
-        <v>0</v>
+        <v>10.60910836007211</v>
       </c>
       <c r="Q52">
         <v>0</v>
@@ -4918,13 +4894,13 @@
         <v>0.219821547433524</v>
       </c>
       <c r="N53">
-        <v>0</v>
+        <v>78.0603527336621</v>
       </c>
       <c r="O53">
         <v>9.677745526743548</v>
       </c>
       <c r="P53">
-        <v>0</v>
+        <v>8.604742086582633</v>
       </c>
       <c r="Q53">
         <v>4.488844653329641</v>
@@ -5004,13 +4980,13 @@
         <v>0.2341116259500335</v>
       </c>
       <c r="N54">
-        <v>0</v>
+        <v>78.10753765339771</v>
       </c>
       <c r="O54">
         <v>9.782311127552351</v>
       </c>
       <c r="P54">
-        <v>0</v>
+        <v>8.587371946560946</v>
       </c>
       <c r="Q54">
         <v>4.476847110882324</v>
@@ -5090,13 +5066,13 @@
         <v>0</v>
       </c>
       <c r="N55">
-        <v>0</v>
+        <v>62.70127981050267</v>
       </c>
       <c r="O55">
         <v>5.917697701306668</v>
       </c>
       <c r="P55">
-        <v>0</v>
+        <v>0.5762332441197436</v>
       </c>
       <c r="Q55">
         <v>0</v>
@@ -5176,13 +5152,13 @@
         <v>0</v>
       </c>
       <c r="N56">
-        <v>0</v>
+        <v>73.7826968708834</v>
       </c>
       <c r="O56">
         <v>3.980286252034801</v>
       </c>
       <c r="P56">
-        <v>0</v>
+        <v>15.41070374272655</v>
       </c>
       <c r="Q56">
         <v>7.16071661374829</v>
@@ -5262,13 +5238,13 @@
         <v>0</v>
       </c>
       <c r="N57">
-        <v>0</v>
+        <v>72.78567923807694</v>
       </c>
       <c r="O57">
         <v>4.114305330849022</v>
       </c>
       <c r="P57">
-        <v>0</v>
+        <v>0.6188982870271988</v>
       </c>
       <c r="Q57">
         <v>0</v>
@@ -5348,13 +5324,13 @@
         <v>0</v>
       </c>
       <c r="N58">
-        <v>0</v>
+        <v>72.64457354779189</v>
       </c>
       <c r="O58">
         <v>3.054656121648415</v>
       </c>
       <c r="P58">
-        <v>0</v>
+        <v>5.379702208748427</v>
       </c>
       <c r="Q58">
         <v>0.3224334453177654</v>
@@ -5434,13 +5410,13 @@
         <v>1.800208140696467</v>
       </c>
       <c r="N59">
-        <v>0</v>
+        <v>77.44141488603549</v>
       </c>
       <c r="O59">
         <v>6.219818581835477</v>
       </c>
       <c r="P59">
-        <v>0</v>
+        <v>5.663469796662925</v>
       </c>
       <c r="Q59">
         <v>2.980023677463922</v>
@@ -5520,7 +5496,7 @@
         <v>0</v>
       </c>
       <c r="N60">
-        <v>0</v>
+        <v>89.84978602745963</v>
       </c>
       <c r="O60">
         <v>10.9350303229275</v>
@@ -5606,13 +5582,13 @@
         <v>0</v>
       </c>
       <c r="N61">
-        <v>0</v>
+        <v>57.60729283910511</v>
       </c>
       <c r="O61">
         <v>3.848063693132056</v>
       </c>
       <c r="P61">
-        <v>0</v>
+        <v>3.319715543828756</v>
       </c>
       <c r="Q61">
         <v>1.137400152942005</v>
@@ -5692,13 +5668,13 @@
         <v>0</v>
       </c>
       <c r="N62">
-        <v>0</v>
+        <v>83.77156673129838</v>
       </c>
       <c r="O62">
         <v>5.545937863616823</v>
       </c>
       <c r="P62">
-        <v>0</v>
+        <v>3.652159515644756</v>
       </c>
       <c r="Q62">
         <v>0</v>
@@ -5778,13 +5754,13 @@
         <v>0</v>
       </c>
       <c r="N63">
-        <v>0</v>
+        <v>75.54134759882272</v>
       </c>
       <c r="O63">
         <v>18.50211438787232</v>
       </c>
       <c r="P63">
-        <v>0</v>
+        <v>0.7628734373745703</v>
       </c>
       <c r="Q63">
         <v>0</v>
@@ -5864,13 +5840,13 @@
         <v>0</v>
       </c>
       <c r="N64">
-        <v>0</v>
+        <v>80.31081154817285</v>
       </c>
       <c r="O64">
         <v>2.177664522822068</v>
       </c>
       <c r="P64">
-        <v>0</v>
+        <v>5.771404724780002</v>
       </c>
       <c r="Q64">
         <v>0.6365480912864507</v>
@@ -5950,13 +5926,13 @@
         <v>0</v>
       </c>
       <c r="N65">
-        <v>0</v>
+        <v>80.51357925473094</v>
       </c>
       <c r="O65">
         <v>5.038062162540139</v>
       </c>
       <c r="P65">
-        <v>0</v>
+        <v>2.968549600150132</v>
       </c>
       <c r="Q65">
         <v>0</v>
@@ -6036,13 +6012,13 @@
         <v>0</v>
       </c>
       <c r="N66">
-        <v>0</v>
+        <v>81.35364044548649</v>
       </c>
       <c r="O66">
         <v>3.557852341616109</v>
       </c>
       <c r="P66">
-        <v>0</v>
+        <v>8.926409174780623</v>
       </c>
       <c r="Q66">
         <v>3.151351674502687</v>
@@ -6122,13 +6098,13 @@
         <v>0</v>
       </c>
       <c r="N67">
-        <v>0</v>
+        <v>81.66280391133517</v>
       </c>
       <c r="O67">
         <v>3.864136064655324</v>
       </c>
       <c r="P67">
-        <v>0</v>
+        <v>8.478769908901098</v>
       </c>
       <c r="Q67">
         <v>2.947043021971288</v>
@@ -6208,13 +6184,13 @@
         <v>0</v>
       </c>
       <c r="N68">
-        <v>0</v>
+        <v>81.02586561773606</v>
       </c>
       <c r="O68">
         <v>1.489598864367927</v>
       </c>
       <c r="P68">
-        <v>0</v>
+        <v>3.354642712832195</v>
       </c>
       <c r="Q68">
         <v>0</v>
@@ -6294,13 +6270,13 @@
         <v>0</v>
       </c>
       <c r="N69">
-        <v>0</v>
+        <v>80.83602300992152</v>
       </c>
       <c r="O69">
         <v>1.637848440529288</v>
       </c>
       <c r="P69">
-        <v>0</v>
+        <v>2.88211730887596</v>
       </c>
       <c r="Q69">
         <v>0</v>
@@ -6380,7 +6356,7 @@
         <v>0</v>
       </c>
       <c r="N70">
-        <v>0</v>
+        <v>84.75392801954621</v>
       </c>
       <c r="O70">
         <v>3.306071700836108</v>
@@ -6466,13 +6442,13 @@
         <v>0</v>
       </c>
       <c r="N71">
-        <v>0</v>
+        <v>79.36640777736228</v>
       </c>
       <c r="O71">
         <v>2.610148852624208</v>
       </c>
       <c r="P71">
-        <v>0</v>
+        <v>6.956236558435129</v>
       </c>
       <c r="Q71">
         <v>0.2802440021352919</v>
@@ -6552,13 +6528,13 @@
         <v>0</v>
       </c>
       <c r="N72">
-        <v>0</v>
+        <v>69.40769697448474</v>
       </c>
       <c r="O72">
         <v>5.891408762001594</v>
       </c>
       <c r="P72">
-        <v>0</v>
+        <v>1.563339657696347</v>
       </c>
       <c r="Q72">
         <v>0</v>
@@ -6638,13 +6614,13 @@
         <v>8.265127248861873</v>
       </c>
       <c r="N73">
-        <v>0</v>
+        <v>56.57476119031467</v>
       </c>
       <c r="O73">
         <v>4.854925824322669</v>
       </c>
       <c r="P73">
-        <v>0</v>
+        <v>1.625090904274282</v>
       </c>
       <c r="Q73">
         <v>0.7529386912608985</v>
@@ -6724,13 +6700,13 @@
         <v>2.400454239445537</v>
       </c>
       <c r="N74">
-        <v>0</v>
+        <v>58.3574281261688</v>
       </c>
       <c r="O74">
         <v>8.915757525339789</v>
       </c>
       <c r="P74">
-        <v>0</v>
+        <v>26.35661774365619</v>
       </c>
       <c r="Q74">
         <v>15.92619185920652</v>
@@ -6810,13 +6786,13 @@
         <v>1.650613948876363</v>
       </c>
       <c r="N75">
-        <v>0</v>
+        <v>79.31594504268541</v>
       </c>
       <c r="O75">
         <v>7.009436022254192</v>
       </c>
       <c r="P75">
-        <v>0</v>
+        <v>4.823912128606558</v>
       </c>
       <c r="Q75">
         <v>2.454291756861483</v>
@@ -6896,13 +6872,13 @@
         <v>18.98049022969667</v>
       </c>
       <c r="N76">
-        <v>0</v>
+        <v>54.81498153925603</v>
       </c>
       <c r="O76">
         <v>5.01913155191336</v>
       </c>
       <c r="P76">
-        <v>0</v>
+        <v>2.551822711517922</v>
       </c>
       <c r="Q76">
         <v>0.855195812444036</v>
@@ -6982,13 +6958,13 @@
         <v>0</v>
       </c>
       <c r="N77">
-        <v>0</v>
+        <v>42.51769026279446</v>
       </c>
       <c r="O77">
         <v>4.860407928343805</v>
       </c>
       <c r="P77">
-        <v>0</v>
+        <v>1.327625311751483</v>
       </c>
       <c r="Q77">
         <v>0</v>
@@ -7068,13 +7044,13 @@
         <v>5.845270540967756</v>
       </c>
       <c r="N78">
-        <v>0</v>
+        <v>73.31951031304369</v>
       </c>
       <c r="O78">
         <v>12.96280454061837</v>
       </c>
       <c r="P78">
-        <v>0</v>
+        <v>1.909342450918183</v>
       </c>
       <c r="Q78">
         <v>0.5624869136068055</v>
@@ -7154,13 +7130,13 @@
         <v>0</v>
       </c>
       <c r="N79">
-        <v>0</v>
+        <v>70.01956507667637</v>
       </c>
       <c r="O79">
         <v>11.19291833781825</v>
       </c>
       <c r="P79">
-        <v>0</v>
+        <v>1.415927912837631</v>
       </c>
       <c r="Q79">
         <v>0.2241404595045615</v>
@@ -7240,13 +7216,13 @@
         <v>0</v>
       </c>
       <c r="N80">
-        <v>0</v>
+        <v>64.37627084029971</v>
       </c>
       <c r="O80">
         <v>57.1676883888893</v>
       </c>
       <c r="P80">
-        <v>0</v>
+        <v>2.938949016908311</v>
       </c>
       <c r="Q80">
         <v>1.677757513737322</v>
@@ -7326,13 +7302,13 @@
         <v>0</v>
       </c>
       <c r="N81">
-        <v>0</v>
+        <v>65.08169326812285</v>
       </c>
       <c r="O81">
         <v>38.14588863704108</v>
       </c>
       <c r="P81">
-        <v>0</v>
+        <v>2.214688872503557</v>
       </c>
       <c r="Q81">
         <v>2.214688872503557</v>
@@ -7412,13 +7388,13 @@
         <v>0</v>
       </c>
       <c r="N82">
-        <v>0</v>
+        <v>53.66788426763996</v>
       </c>
       <c r="O82">
         <v>24.7780923571811</v>
       </c>
       <c r="P82">
-        <v>0</v>
+        <v>10.34668835148259</v>
       </c>
       <c r="Q82">
         <v>1.427643205769132</v>
@@ -7498,13 +7474,13 @@
         <v>0</v>
       </c>
       <c r="N83">
-        <v>0</v>
+        <v>68.24656531335694</v>
       </c>
       <c r="O83">
         <v>48.2787889822618</v>
       </c>
       <c r="P83">
-        <v>0</v>
+        <v>11.3285785113237</v>
       </c>
       <c r="Q83">
         <v>6.436803400380454</v>
@@ -7584,13 +7560,13 @@
         <v>0</v>
       </c>
       <c r="N84">
-        <v>0</v>
+        <v>77.31182186132298</v>
       </c>
       <c r="O84">
         <v>44.67188490747676</v>
       </c>
       <c r="P84">
-        <v>0</v>
+        <v>1.779698211041209</v>
       </c>
       <c r="Q84">
         <v>0</v>
@@ -7670,13 +7646,13 @@
         <v>0</v>
       </c>
       <c r="N85">
-        <v>0</v>
+        <v>70.76318843203714</v>
       </c>
       <c r="O85">
         <v>52.54450209216831</v>
       </c>
       <c r="P85">
-        <v>0</v>
+        <v>5.732983613553893</v>
       </c>
       <c r="Q85">
         <v>3.224519976726511</v>
@@ -7756,7 +7732,7 @@
         <v>0</v>
       </c>
       <c r="N86">
-        <v>0</v>
+        <v>88.08895632972508</v>
       </c>
       <c r="O86">
         <v>25.05796193883537</v>
@@ -7842,7 +7818,7 @@
         <v>0</v>
       </c>
       <c r="N87">
-        <v>0</v>
+        <v>63.21017357998198</v>
       </c>
       <c r="O87">
         <v>0</v>
@@ -7928,7 +7904,7 @@
         <v>0</v>
       </c>
       <c r="N88">
-        <v>0</v>
+        <v>89.53843849645025</v>
       </c>
       <c r="O88">
         <v>12.04429412268748</v>
@@ -8014,7 +7990,7 @@
         <v>0</v>
       </c>
       <c r="N89">
-        <v>0</v>
+        <v>87.80157322331155</v>
       </c>
       <c r="O89">
         <v>1.35680240339036</v>
@@ -8100,7 +8076,7 @@
         <v>0</v>
       </c>
       <c r="N90">
-        <v>0</v>
+        <v>86.97194553891732</v>
       </c>
       <c r="O90">
         <v>13.65992684704628</v>
@@ -8186,7 +8162,7 @@
         <v>0</v>
       </c>
       <c r="N91">
-        <v>0</v>
+        <v>84.39556873425781</v>
       </c>
       <c r="O91">
         <v>11.86205602521186</v>
@@ -8272,7 +8248,7 @@
         <v>0</v>
       </c>
       <c r="N92">
-        <v>0</v>
+        <v>78.87482691925524</v>
       </c>
       <c r="O92">
         <v>2.32130784086785</v>
@@ -8358,7 +8334,7 @@
         <v>0</v>
       </c>
       <c r="N93">
-        <v>0</v>
+        <v>81.39548788302689</v>
       </c>
       <c r="O93">
         <v>8.477313342177661</v>
@@ -8444,7 +8420,7 @@
         <v>0</v>
       </c>
       <c r="N94">
-        <v>0</v>
+        <v>85.82377923024782</v>
       </c>
       <c r="O94">
         <v>3.093818355017319</v>
@@ -8530,7 +8506,7 @@
         <v>0</v>
       </c>
       <c r="N95">
-        <v>0</v>
+        <v>79.34972802352885</v>
       </c>
       <c r="O95">
         <v>4.511471579579979</v>
@@ -8616,7 +8592,7 @@
         <v>0</v>
       </c>
       <c r="N96">
-        <v>0</v>
+        <v>77.59021549947485</v>
       </c>
       <c r="O96">
         <v>5.620270468374463</v>
@@ -8702,7 +8678,7 @@
         <v>0</v>
       </c>
       <c r="N97">
-        <v>0</v>
+        <v>82.46348349757557</v>
       </c>
       <c r="O97">
         <v>9.38327672572041</v>
@@ -8788,7 +8764,7 @@
         <v>0</v>
       </c>
       <c r="N98">
-        <v>0</v>
+        <v>89.67369157786214</v>
       </c>
       <c r="O98">
         <v>50.51118751804496</v>
@@ -8874,7 +8850,7 @@
         <v>0</v>
       </c>
       <c r="N99">
-        <v>0</v>
+        <v>75.4082587056395</v>
       </c>
       <c r="O99">
         <v>4.215492041223614</v>
@@ -8960,7 +8936,7 @@
         <v>0</v>
       </c>
       <c r="N100">
-        <v>0</v>
+        <v>91.59842507420005</v>
       </c>
       <c r="O100">
         <v>26.29696803466321</v>
@@ -9046,7 +9022,7 @@
         <v>0</v>
       </c>
       <c r="N101">
-        <v>0</v>
+        <v>85.52631504320564</v>
       </c>
       <c r="O101">
         <v>49.02815470987321</v>
@@ -9132,7 +9108,7 @@
         <v>0</v>
       </c>
       <c r="N102">
-        <v>0</v>
+        <v>87.53271996858494</v>
       </c>
       <c r="O102">
         <v>0.04953660767144213</v>
@@ -9218,7 +9194,7 @@
         <v>0</v>
       </c>
       <c r="N103">
-        <v>0</v>
+        <v>78.62836222930245</v>
       </c>
       <c r="O103">
         <v>0</v>
@@ -9304,7 +9280,7 @@
         <v>0</v>
       </c>
       <c r="N104">
-        <v>0</v>
+        <v>83.90312425707026</v>
       </c>
       <c r="O104">
         <v>20.1789537277666</v>
@@ -9390,7 +9366,7 @@
         <v>0</v>
       </c>
       <c r="N105">
-        <v>0</v>
+        <v>86.96629571490303</v>
       </c>
       <c r="O105">
         <v>86.96629571490303</v>
@@ -9476,7 +9452,7 @@
         <v>0</v>
       </c>
       <c r="N106">
-        <v>0</v>
+        <v>92.08464293640768</v>
       </c>
       <c r="O106">
         <v>5.775341054832954</v>
@@ -9562,7 +9538,7 @@
         <v>0</v>
       </c>
       <c r="N107">
-        <v>0</v>
+        <v>76.55407097629603</v>
       </c>
       <c r="O107">
         <v>3.073051683346461</v>
@@ -9648,7 +9624,7 @@
         <v>0</v>
       </c>
       <c r="N108">
-        <v>0</v>
+        <v>59.6925854304729</v>
       </c>
       <c r="O108">
         <v>5.222720074025041</v>
@@ -9734,7 +9710,7 @@
         <v>0</v>
       </c>
       <c r="N109">
-        <v>0</v>
+        <v>76.9384191063113</v>
       </c>
       <c r="O109">
         <v>5.983771508770753</v>
@@ -9820,7 +9796,7 @@
         <v>0</v>
       </c>
       <c r="N110">
-        <v>0</v>
+        <v>70.5498431148126</v>
       </c>
       <c r="O110">
         <v>20.31005601799485</v>
@@ -9906,7 +9882,7 @@
         <v>0</v>
       </c>
       <c r="N111">
-        <v>0</v>
+        <v>74.70104505125212</v>
       </c>
       <c r="O111">
         <v>3.78833724092939</v>
@@ -9992,7 +9968,7 @@
         <v>0</v>
       </c>
       <c r="N112">
-        <v>0</v>
+        <v>76.45526230819705</v>
       </c>
       <c r="O112">
         <v>5.455874351563859</v>
@@ -10078,7 +10054,7 @@
         <v>0</v>
       </c>
       <c r="N113">
-        <v>0</v>
+        <v>86.11737308419762</v>
       </c>
       <c r="O113">
         <v>10.89439993260421</v>
@@ -10164,7 +10140,7 @@
         <v>0</v>
       </c>
       <c r="N114">
-        <v>0</v>
+        <v>87.37160308877111</v>
       </c>
       <c r="O114">
         <v>12.6571732692556</v>
@@ -10250,7 +10226,7 @@
         <v>0</v>
       </c>
       <c r="N115">
-        <v>0</v>
+        <v>92.28604127808728</v>
       </c>
       <c r="O115">
         <v>3.222865298225244</v>
@@ -10336,7 +10312,7 @@
         <v>0</v>
       </c>
       <c r="N116">
-        <v>0</v>
+        <v>81.91588842512147</v>
       </c>
       <c r="O116">
         <v>0</v>
@@ -11190,7 +11166,7 @@
         <v>0</v>
       </c>
       <c r="N126">
-        <v>66.23999999999999</v>
+        <v>66.239</v>
       </c>
       <c r="O126">
         <v>55.903</v>
@@ -11362,7 +11338,7 @@
         <v>0.018</v>
       </c>
       <c r="N128">
-        <v>58.118</v>
+        <v>58.11799999999999</v>
       </c>
       <c r="O128">
         <v>46.354</v>
@@ -11448,7 +11424,7 @@
         <v>0</v>
       </c>
       <c r="N129">
-        <v>80.40900000000001</v>
+        <v>80.40899999999999</v>
       </c>
       <c r="O129">
         <v>80.267</v>
@@ -11542,15 +11518,6 @@
       <c r="P130">
         <v>10.062</v>
       </c>
-      <c r="Q130">
-        <v>0</v>
-      </c>
-      <c r="R130">
-        <v>0</v>
-      </c>
-      <c r="S130">
-        <v>0</v>
-      </c>
       <c r="T130">
         <v>6.745</v>
       </c>
@@ -11620,22 +11587,13 @@
         <v>3.785</v>
       </c>
       <c r="N131">
-        <v>77.586</v>
+        <v>77.587</v>
       </c>
       <c r="O131">
         <v>62.291</v>
       </c>
       <c r="P131">
         <v>1.458</v>
-      </c>
-      <c r="Q131">
-        <v>0</v>
-      </c>
-      <c r="R131">
-        <v>0</v>
-      </c>
-      <c r="S131">
-        <v>0</v>
       </c>
       <c r="T131">
         <v>3.233</v>
@@ -11964,7 +11922,7 @@
         <v>0.063</v>
       </c>
       <c r="N135">
-        <v>72.538</v>
+        <v>72.539</v>
       </c>
       <c r="O135">
         <v>65.27200000000001</v>
@@ -12566,7 +12524,7 @@
         <v>0.478</v>
       </c>
       <c r="N142">
-        <v>59.056</v>
+        <v>59.055</v>
       </c>
       <c r="O142">
         <v>47.524</v>
@@ -12746,15 +12704,6 @@
       <c r="P144">
         <v>0.281</v>
       </c>
-      <c r="Q144">
-        <v>0</v>
-      </c>
-      <c r="R144">
-        <v>0</v>
-      </c>
-      <c r="S144">
-        <v>0</v>
-      </c>
       <c r="T144">
         <v>7.522</v>
       </c>
@@ -12832,15 +12781,6 @@
       <c r="P145">
         <v>3.681</v>
       </c>
-      <c r="Q145">
-        <v>0</v>
-      </c>
-      <c r="R145">
-        <v>0</v>
-      </c>
-      <c r="S145">
-        <v>0</v>
-      </c>
       <c r="T145">
         <v>1.206</v>
       </c>
@@ -13168,7 +13108,7 @@
         <v>0.65</v>
       </c>
       <c r="N149">
-        <v>80.27500000000001</v>
+        <v>80.27399999999999</v>
       </c>
       <c r="O149">
         <v>69.06399999999999</v>
@@ -13254,7 +13194,7 @@
         <v>0</v>
       </c>
       <c r="N150">
-        <v>76.605</v>
+        <v>76.60400000000001</v>
       </c>
       <c r="O150">
         <v>52.423</v>
@@ -13340,7 +13280,7 @@
         <v>0</v>
       </c>
       <c r="N151">
-        <v>72.616</v>
+        <v>72.61600000000001</v>
       </c>
       <c r="O151">
         <v>54.938</v>
@@ -13942,7 +13882,7 @@
         <v>0</v>
       </c>
       <c r="N158">
-        <v>95.90000000000001</v>
+        <v>95.89999999999999</v>
       </c>
       <c r="O158">
         <v>89.3</v>
@@ -15066,7 +15006,7 @@
         <v>61.3</v>
       </c>
       <c r="P171">
-        <v>9.1</v>
+        <v>9.100000000000001</v>
       </c>
       <c r="Q171">
         <v>8.800000000000001</v>
@@ -16439,7 +16379,7 @@
         <v>19.643</v>
       </c>
       <c r="P187">
-        <v>48.556</v>
+        <v>48.557</v>
       </c>
       <c r="Q187">
         <v>18.374</v>
@@ -16825,7 +16765,7 @@
         <v>0</v>
       </c>
       <c r="N194">
-        <v>2.735</v>
+        <v>2.736</v>
       </c>
       <c r="O194">
         <v>0</v>
@@ -17177,7 +17117,7 @@
         <v>0</v>
       </c>
       <c r="P199">
-        <v>33.674</v>
+        <v>33.673</v>
       </c>
       <c r="Q199">
         <v>0</v>
@@ -19149,7 +19089,7 @@
         <v>37.147</v>
       </c>
       <c r="N222">
-        <v>40.895</v>
+        <v>40.894</v>
       </c>
       <c r="O222">
         <v>11.406</v>
@@ -19235,7 +19175,7 @@
         <v>44.866</v>
       </c>
       <c r="N223">
-        <v>37.471</v>
+        <v>37.47</v>
       </c>
       <c r="O223">
         <v>1.842</v>
@@ -19321,7 +19261,7 @@
         <v>0</v>
       </c>
       <c r="N224">
-        <v>8.808</v>
+        <v>8.807</v>
       </c>
       <c r="O224">
         <v>8.380000000000001</v>
@@ -20269,7 +20209,7 @@
         <v>2.172</v>
       </c>
       <c r="N236">
-        <v>75.435</v>
+        <v>75.43600000000001</v>
       </c>
       <c r="O236">
         <v>68.02800000000001</v>
@@ -20441,7 +20381,7 @@
         <v>0.765</v>
       </c>
       <c r="N238">
-        <v>86.42700000000001</v>
+        <v>86.42600000000002</v>
       </c>
       <c r="O238">
         <v>63.026</v>
@@ -20785,7 +20725,7 @@
         <v>2.42</v>
       </c>
       <c r="N242">
-        <v>67.42</v>
+        <v>67.42100000000001</v>
       </c>
       <c r="O242">
         <v>0.231</v>
@@ -20957,7 +20897,7 @@
         <v>1.076</v>
       </c>
       <c r="N244">
-        <v>25.025</v>
+        <v>25.024</v>
       </c>
       <c r="O244">
         <v>5.657</v>
@@ -21215,7 +21155,7 @@
         <v>2.445</v>
       </c>
       <c r="N247">
-        <v>5.506</v>
+        <v>5.505</v>
       </c>
       <c r="O247">
         <v>0</v>
@@ -22247,7 +22187,7 @@
         <v>0</v>
       </c>
       <c r="N259">
-        <v>19.236</v>
+        <v>19.237</v>
       </c>
       <c r="O259">
         <v>0.161</v>
@@ -22668,7 +22608,7 @@
         <v>4.964</v>
       </c>
       <c r="N264">
-        <v>73.89700000000001</v>
+        <v>73.89699999999999</v>
       </c>
       <c r="O264">
         <v>63.58</v>
@@ -22917,22 +22857,13 @@
         <v>0</v>
       </c>
       <c r="N267">
-        <v>82.295</v>
+        <v>82.29499999999999</v>
       </c>
       <c r="O267">
         <v>80.77</v>
       </c>
       <c r="P267">
         <v>0.834</v>
-      </c>
-      <c r="Q267">
-        <v>0</v>
-      </c>
-      <c r="R267">
-        <v>0</v>
-      </c>
-      <c r="S267">
-        <v>0</v>
       </c>
       <c r="T267">
         <v>1.873</v>
@@ -23097,15 +23028,6 @@
       <c r="P269">
         <v>46.037</v>
       </c>
-      <c r="Q269">
-        <v>0</v>
-      </c>
-      <c r="R269">
-        <v>0</v>
-      </c>
-      <c r="S269">
-        <v>0</v>
-      </c>
       <c r="T269">
         <v>5.985</v>
       </c>
@@ -23175,7 +23097,7 @@
         <v>0.8129999999999999</v>
       </c>
       <c r="N270">
-        <v>62.082</v>
+        <v>62.08300000000001</v>
       </c>
       <c r="O270">
         <v>49.948</v>
@@ -23424,7 +23346,7 @@
         <v>1.012</v>
       </c>
       <c r="N273">
-        <v>81.30500000000001</v>
+        <v>81.30499999999999</v>
       </c>
       <c r="O273">
         <v>59.3</v>
@@ -23501,22 +23423,13 @@
         <v>0</v>
       </c>
       <c r="N274">
-        <v>76.333</v>
+        <v>76.33200000000001</v>
       </c>
       <c r="O274">
         <v>73.429</v>
       </c>
       <c r="P274">
         <v>3.404</v>
-      </c>
-      <c r="Q274">
-        <v>0</v>
-      </c>
-      <c r="R274">
-        <v>0</v>
-      </c>
-      <c r="S274">
-        <v>0</v>
       </c>
       <c r="T274">
         <v>19.329</v>
@@ -23587,7 +23500,7 @@
         <v>0</v>
       </c>
       <c r="N275">
-        <v>80.40900000000001</v>
+        <v>80.40799999999999</v>
       </c>
       <c r="O275">
         <v>75.877</v>
@@ -23664,22 +23577,13 @@
         <v>0</v>
       </c>
       <c r="N276">
-        <v>59.154</v>
+        <v>59.153</v>
       </c>
       <c r="O276">
         <v>49.669</v>
       </c>
       <c r="P276">
         <v>0.341</v>
-      </c>
-      <c r="Q276">
-        <v>0</v>
-      </c>
-      <c r="R276">
-        <v>0</v>
-      </c>
-      <c r="S276">
-        <v>0</v>
       </c>
       <c r="T276">
         <v>20.632</v>
@@ -23836,7 +23740,7 @@
         <v>0</v>
       </c>
       <c r="N278">
-        <v>5.275</v>
+        <v>5.276</v>
       </c>
       <c r="O278">
         <v>0</v>
@@ -23930,15 +23834,6 @@
       <c r="P279">
         <v>4.568</v>
       </c>
-      <c r="Q279">
-        <v>0</v>
-      </c>
-      <c r="R279">
-        <v>0</v>
-      </c>
-      <c r="S279">
-        <v>0</v>
-      </c>
       <c r="T279">
         <v>39.918</v>
       </c>
@@ -24008,7 +23903,7 @@
         <v>0</v>
       </c>
       <c r="N280">
-        <v>19.596</v>
+        <v>19.597</v>
       </c>
       <c r="O280">
         <v>18.374</v>
@@ -24085,7 +23980,7 @@
         <v>0</v>
       </c>
       <c r="N281">
-        <v>75.943</v>
+        <v>75.94300000000001</v>
       </c>
       <c r="O281">
         <v>73.04300000000001</v>
@@ -24429,7 +24324,7 @@
         <v>0.429</v>
       </c>
       <c r="N285">
-        <v>78.22</v>
+        <v>78.22000000000001</v>
       </c>
       <c r="O285">
         <v>77.68000000000001</v>
@@ -24773,7 +24668,7 @@
         <v>0</v>
       </c>
       <c r="N289">
-        <v>78.315</v>
+        <v>78.31500000000001</v>
       </c>
       <c r="O289">
         <v>77.77500000000001</v>
@@ -24859,7 +24754,7 @@
         <v>0</v>
       </c>
       <c r="N290">
-        <v>74.767</v>
+        <v>74.768</v>
       </c>
       <c r="O290">
         <v>74.761</v>
@@ -25203,7 +25098,7 @@
         <v>0</v>
       </c>
       <c r="N294">
-        <v>73.366</v>
+        <v>73.367</v>
       </c>
       <c r="O294">
         <v>63.685</v>
@@ -25289,7 +25184,7 @@
         <v>0</v>
       </c>
       <c r="N295">
-        <v>79.169</v>
+        <v>79.16900000000001</v>
       </c>
       <c r="O295">
         <v>77.39100000000001</v>
@@ -25375,7 +25270,7 @@
         <v>0</v>
       </c>
       <c r="N296">
-        <v>85.97799999999999</v>
+        <v>85.97800000000001</v>
       </c>
       <c r="O296">
         <v>79.02500000000001</v>
@@ -26579,7 +26474,7 @@
         <v>0</v>
       </c>
       <c r="N310">
-        <v>47.981</v>
+        <v>47.982</v>
       </c>
       <c r="O310">
         <v>10.382</v>
@@ -26751,7 +26646,7 @@
         <v>0</v>
       </c>
       <c r="N312">
-        <v>80.324</v>
+        <v>80.32400000000001</v>
       </c>
       <c r="O312">
         <v>80.28400000000001</v>
@@ -26837,7 +26732,7 @@
         <v>0.93</v>
       </c>
       <c r="N313">
-        <v>3.437</v>
+        <v>3.436</v>
       </c>
       <c r="O313">
         <v>0</v>
@@ -27009,7 +26904,7 @@
         <v>0</v>
       </c>
       <c r="N315">
-        <v>65.46599999999999</v>
+        <v>65.467</v>
       </c>
       <c r="O315">
         <v>30.378</v>
@@ -27353,13 +27248,13 @@
         <v>8.878</v>
       </c>
       <c r="N319">
-        <v>74.182</v>
+        <v>74.18199999999999</v>
       </c>
       <c r="O319">
         <v>58.236</v>
       </c>
       <c r="P319">
-        <v>1.133</v>
+        <v>1.132</v>
       </c>
       <c r="Q319">
         <v>1.075</v>
@@ -27525,7 +27420,7 @@
         <v>2.1</v>
       </c>
       <c r="N321">
-        <v>68.72799999999999</v>
+        <v>68.727</v>
       </c>
       <c r="O321">
         <v>59.109</v>
@@ -27789,7 +27684,7 @@
         <v>0</v>
       </c>
       <c r="P324">
-        <v>17.507</v>
+        <v>17.506</v>
       </c>
       <c r="Q324">
         <v>14.322</v>
@@ -28391,7 +28286,7 @@
         <v>0</v>
       </c>
       <c r="P331">
-        <v>49.755</v>
+        <v>49.754</v>
       </c>
       <c r="Q331">
         <v>48.772</v>
@@ -28477,7 +28372,7 @@
         <v>0</v>
       </c>
       <c r="P332">
-        <v>54.753</v>
+        <v>54.754</v>
       </c>
       <c r="Q332">
         <v>48.45</v>
@@ -29167,15 +29062,6 @@
       <c r="P340">
         <v>55.874</v>
       </c>
-      <c r="Q340">
-        <v>0</v>
-      </c>
-      <c r="R340">
-        <v>0</v>
-      </c>
-      <c r="S340">
-        <v>0</v>
-      </c>
       <c r="T340">
         <v>0.636</v>
       </c>
@@ -29245,22 +29131,13 @@
         <v>1.512</v>
       </c>
       <c r="N341">
-        <v>83.812</v>
+        <v>83.81200000000001</v>
       </c>
       <c r="O341">
         <v>68.16200000000001</v>
       </c>
       <c r="P341">
         <v>2.608</v>
-      </c>
-      <c r="Q341">
-        <v>0</v>
-      </c>
-      <c r="R341">
-        <v>0</v>
-      </c>
-      <c r="S341">
-        <v>0</v>
       </c>
       <c r="T341">
         <v>3.007</v>
@@ -29331,22 +29208,13 @@
         <v>10.446</v>
       </c>
       <c r="N342">
-        <v>50.135</v>
+        <v>50.136</v>
       </c>
       <c r="O342">
         <v>29.794</v>
       </c>
       <c r="P342">
         <v>6.468</v>
-      </c>
-      <c r="Q342">
-        <v>0</v>
-      </c>
-      <c r="R342">
-        <v>0</v>
-      </c>
-      <c r="S342">
-        <v>0</v>
       </c>
       <c r="T342">
         <v>0.276</v>
@@ -29417,7 +29285,7 @@
         <v>0.141</v>
       </c>
       <c r="N343">
-        <v>75.005</v>
+        <v>75.006</v>
       </c>
       <c r="O343">
         <v>71.087</v>
@@ -29502,15 +29370,6 @@
       <c r="P344">
         <v>0.333</v>
       </c>
-      <c r="Q344">
-        <v>0</v>
-      </c>
-      <c r="R344">
-        <v>0</v>
-      </c>
-      <c r="S344">
-        <v>0</v>
-      </c>
       <c r="T344">
         <v>10.878</v>
       </c>
@@ -29580,7 +29439,7 @@
         <v>0</v>
       </c>
       <c r="N345">
-        <v>63.511</v>
+        <v>63.512</v>
       </c>
       <c r="O345">
         <v>2.792</v>
@@ -29924,22 +29783,13 @@
         <v>0.494</v>
       </c>
       <c r="N349">
-        <v>80.48</v>
+        <v>80.479</v>
       </c>
       <c r="O349">
         <v>65.70999999999999</v>
       </c>
       <c r="P349">
         <v>1.393</v>
-      </c>
-      <c r="Q349">
-        <v>0</v>
-      </c>
-      <c r="R349">
-        <v>0</v>
-      </c>
-      <c r="S349">
-        <v>0</v>
       </c>
       <c r="T349">
         <v>6.26</v>
@@ -30018,15 +29868,6 @@
       <c r="P350">
         <v>1.859</v>
       </c>
-      <c r="Q350">
-        <v>0</v>
-      </c>
-      <c r="R350">
-        <v>0</v>
-      </c>
-      <c r="S350">
-        <v>0</v>
-      </c>
       <c r="T350">
         <v>6.331</v>
       </c>
@@ -30096,22 +29937,13 @@
         <v>0.136</v>
       </c>
       <c r="N351">
-        <v>70.907</v>
+        <v>70.90600000000001</v>
       </c>
       <c r="O351">
         <v>64.229</v>
       </c>
       <c r="P351">
         <v>0.234</v>
-      </c>
-      <c r="Q351">
-        <v>0</v>
-      </c>
-      <c r="R351">
-        <v>0</v>
-      </c>
-      <c r="S351">
-        <v>0</v>
       </c>
       <c r="T351">
         <v>0.124</v>
@@ -30182,22 +30014,13 @@
         <v>1.186</v>
       </c>
       <c r="N352">
-        <v>74.508</v>
+        <v>74.50800000000001</v>
       </c>
       <c r="O352">
         <v>73.179</v>
       </c>
       <c r="P352">
         <v>1.002</v>
-      </c>
-      <c r="Q352">
-        <v>0</v>
-      </c>
-      <c r="R352">
-        <v>0</v>
-      </c>
-      <c r="S352">
-        <v>0</v>
       </c>
       <c r="T352">
         <v>4.513</v>
@@ -30268,22 +30091,13 @@
         <v>0.055</v>
       </c>
       <c r="N353">
-        <v>74.06999999999999</v>
+        <v>74.069</v>
       </c>
       <c r="O353">
         <v>73.227</v>
       </c>
       <c r="P353">
         <v>1.061</v>
-      </c>
-      <c r="Q353">
-        <v>0</v>
-      </c>
-      <c r="R353">
-        <v>0</v>
-      </c>
-      <c r="S353">
-        <v>0</v>
       </c>
       <c r="T353">
         <v>2.183</v>
@@ -30354,22 +30168,13 @@
         <v>0</v>
       </c>
       <c r="N354">
-        <v>79.06399999999999</v>
+        <v>79.06400000000001</v>
       </c>
       <c r="O354">
         <v>77.697</v>
       </c>
       <c r="P354">
         <v>0.328</v>
-      </c>
-      <c r="Q354">
-        <v>0</v>
-      </c>
-      <c r="R354">
-        <v>0</v>
-      </c>
-      <c r="S354">
-        <v>0</v>
       </c>
       <c r="T354">
         <v>5.7</v>
@@ -30440,22 +30245,13 @@
         <v>0.296</v>
       </c>
       <c r="N355">
-        <v>80.437</v>
+        <v>80.43599999999999</v>
       </c>
       <c r="O355">
         <v>68.389</v>
       </c>
       <c r="P355">
         <v>0.971</v>
-      </c>
-      <c r="Q355">
-        <v>0</v>
-      </c>
-      <c r="R355">
-        <v>0</v>
-      </c>
-      <c r="S355">
-        <v>0</v>
       </c>
       <c r="T355">
         <v>5.734</v>
@@ -30534,15 +30330,6 @@
       <c r="P356">
         <v>1.865</v>
       </c>
-      <c r="Q356">
-        <v>0</v>
-      </c>
-      <c r="R356">
-        <v>0</v>
-      </c>
-      <c r="S356">
-        <v>0</v>
-      </c>
       <c r="T356">
         <v>1.19</v>
       </c>
@@ -30706,15 +30493,6 @@
       <c r="P358">
         <v>1.172</v>
       </c>
-      <c r="Q358">
-        <v>0</v>
-      </c>
-      <c r="R358">
-        <v>0</v>
-      </c>
-      <c r="S358">
-        <v>0</v>
-      </c>
       <c r="T358">
         <v>3.508</v>
       </c>
@@ -30784,22 +30562,13 @@
         <v>0.078</v>
       </c>
       <c r="N359">
-        <v>87.542</v>
+        <v>87.54199999999999</v>
       </c>
       <c r="O359">
         <v>82.72</v>
       </c>
       <c r="P359">
         <v>0.697</v>
-      </c>
-      <c r="Q359">
-        <v>0</v>
-      </c>
-      <c r="R359">
-        <v>0</v>
-      </c>
-      <c r="S359">
-        <v>0</v>
       </c>
       <c r="T359">
         <v>5.306</v>
@@ -30956,22 +30725,13 @@
         <v>0</v>
       </c>
       <c r="N361">
-        <v>85.215</v>
+        <v>85.21499999999999</v>
       </c>
       <c r="O361">
         <v>79.008</v>
       </c>
       <c r="P361">
         <v>2.088</v>
-      </c>
-      <c r="Q361">
-        <v>0</v>
-      </c>
-      <c r="R361">
-        <v>0</v>
-      </c>
-      <c r="S361">
-        <v>0</v>
       </c>
       <c r="T361">
         <v>1.851</v>
@@ -31042,22 +30802,13 @@
         <v>0.789</v>
       </c>
       <c r="N362">
-        <v>78.191</v>
+        <v>78.19099999999999</v>
       </c>
       <c r="O362">
         <v>63.168</v>
       </c>
       <c r="P362">
         <v>5.121</v>
-      </c>
-      <c r="Q362">
-        <v>0</v>
-      </c>
-      <c r="R362">
-        <v>0</v>
-      </c>
-      <c r="S362">
-        <v>0</v>
       </c>
       <c r="T362">
         <v>11.501</v>
@@ -31222,15 +30973,6 @@
       <c r="P364">
         <v>0.254</v>
       </c>
-      <c r="Q364">
-        <v>0</v>
-      </c>
-      <c r="R364">
-        <v>0</v>
-      </c>
-      <c r="S364">
-        <v>0</v>
-      </c>
       <c r="T364">
         <v>5.39</v>
       </c>
@@ -31300,22 +31042,13 @@
         <v>8.954000000000001</v>
       </c>
       <c r="N365">
-        <v>77.279</v>
+        <v>77.28</v>
       </c>
       <c r="O365">
         <v>68.863</v>
       </c>
       <c r="P365">
         <v>2.444</v>
-      </c>
-      <c r="Q365">
-        <v>0</v>
-      </c>
-      <c r="R365">
-        <v>0</v>
-      </c>
-      <c r="S365">
-        <v>0</v>
       </c>
       <c r="T365">
         <v>0.773</v>
@@ -31394,15 +31127,6 @@
       <c r="P366">
         <v>1.758</v>
       </c>
-      <c r="Q366">
-        <v>0</v>
-      </c>
-      <c r="R366">
-        <v>0</v>
-      </c>
-      <c r="S366">
-        <v>0</v>
-      </c>
       <c r="T366">
         <v>1.204</v>
       </c>
@@ -31472,22 +31196,13 @@
         <v>5.276</v>
       </c>
       <c r="N367">
-        <v>79.48399999999999</v>
+        <v>79.483</v>
       </c>
       <c r="O367">
         <v>66.57299999999999</v>
       </c>
       <c r="P367">
         <v>1.009</v>
-      </c>
-      <c r="Q367">
-        <v>0</v>
-      </c>
-      <c r="R367">
-        <v>0</v>
-      </c>
-      <c r="S367">
-        <v>0</v>
       </c>
       <c r="T367">
         <v>7.458</v>
@@ -31558,22 +31273,13 @@
         <v>0.62</v>
       </c>
       <c r="N368">
-        <v>79.151</v>
+        <v>79.15199999999999</v>
       </c>
       <c r="O368">
         <v>69.163</v>
       </c>
       <c r="P368">
         <v>3.087</v>
-      </c>
-      <c r="Q368">
-        <v>0</v>
-      </c>
-      <c r="R368">
-        <v>0</v>
-      </c>
-      <c r="S368">
-        <v>0</v>
       </c>
       <c r="T368">
         <v>8.988</v>
@@ -31644,22 +31350,13 @@
         <v>0.023</v>
       </c>
       <c r="N369">
-        <v>89.42100000000001</v>
+        <v>89.41999999999999</v>
       </c>
       <c r="O369">
         <v>88.10599999999999</v>
       </c>
       <c r="P369">
         <v>0.213</v>
-      </c>
-      <c r="Q369">
-        <v>0</v>
-      </c>
-      <c r="R369">
-        <v>0</v>
-      </c>
-      <c r="S369">
-        <v>0</v>
       </c>
       <c r="T369">
         <v>1.31</v>
@@ -31738,15 +31435,6 @@
       <c r="P370">
         <v>0.456</v>
       </c>
-      <c r="Q370">
-        <v>0</v>
-      </c>
-      <c r="R370">
-        <v>0</v>
-      </c>
-      <c r="S370">
-        <v>0</v>
-      </c>
       <c r="T370">
         <v>0.643</v>
       </c>
@@ -31816,22 +31504,13 @@
         <v>0.136</v>
       </c>
       <c r="N371">
-        <v>81.553</v>
+        <v>81.55300000000001</v>
       </c>
       <c r="O371">
         <v>67.596</v>
       </c>
       <c r="P371">
         <v>0.961</v>
-      </c>
-      <c r="Q371">
-        <v>0</v>
-      </c>
-      <c r="R371">
-        <v>0</v>
-      </c>
-      <c r="S371">
-        <v>0</v>
       </c>
       <c r="T371">
         <v>1.03</v>
@@ -31902,22 +31581,13 @@
         <v>0</v>
       </c>
       <c r="N372">
-        <v>83.78400000000001</v>
+        <v>83.78399999999999</v>
       </c>
       <c r="O372">
         <v>79.20099999999999</v>
       </c>
       <c r="P372">
         <v>2.065</v>
-      </c>
-      <c r="Q372">
-        <v>0</v>
-      </c>
-      <c r="R372">
-        <v>0</v>
-      </c>
-      <c r="S372">
-        <v>0</v>
       </c>
       <c r="T372">
         <v>0.342</v>
@@ -31988,22 +31658,13 @@
         <v>0</v>
       </c>
       <c r="N373">
-        <v>66.68899999999999</v>
+        <v>66.688</v>
       </c>
       <c r="O373">
         <v>56.643</v>
       </c>
       <c r="P373">
         <v>0.217</v>
-      </c>
-      <c r="Q373">
-        <v>0</v>
-      </c>
-      <c r="R373">
-        <v>0</v>
-      </c>
-      <c r="S373">
-        <v>0</v>
       </c>
       <c r="T373">
         <v>17.532</v>
@@ -32074,22 +31735,13 @@
         <v>1.043</v>
       </c>
       <c r="N374">
-        <v>82.762</v>
+        <v>82.76300000000001</v>
       </c>
       <c r="O374">
         <v>63.234</v>
       </c>
       <c r="P374">
         <v>1.692</v>
-      </c>
-      <c r="Q374">
-        <v>0</v>
-      </c>
-      <c r="R374">
-        <v>0</v>
-      </c>
-      <c r="S374">
-        <v>0</v>
       </c>
       <c r="T374">
         <v>0.293</v>
@@ -32160,22 +31812,13 @@
         <v>0.382</v>
       </c>
       <c r="N375">
-        <v>84.432</v>
+        <v>84.43199999999999</v>
       </c>
       <c r="O375">
         <v>79.026</v>
       </c>
       <c r="P375">
         <v>0.418</v>
-      </c>
-      <c r="Q375">
-        <v>0</v>
-      </c>
-      <c r="R375">
-        <v>0</v>
-      </c>
-      <c r="S375">
-        <v>0</v>
       </c>
       <c r="T375">
         <v>3.578</v>
@@ -32254,15 +31897,6 @@
       <c r="P376">
         <v>2.157</v>
       </c>
-      <c r="Q376">
-        <v>0</v>
-      </c>
-      <c r="R376">
-        <v>0</v>
-      </c>
-      <c r="S376">
-        <v>0</v>
-      </c>
       <c r="T376">
         <v>4.222</v>
       </c>
@@ -32340,15 +31974,6 @@
       <c r="P377">
         <v>0.217</v>
       </c>
-      <c r="Q377">
-        <v>0</v>
-      </c>
-      <c r="R377">
-        <v>0</v>
-      </c>
-      <c r="S377">
-        <v>0</v>
-      </c>
       <c r="T377">
         <v>10.23</v>
       </c>
@@ -32426,15 +32051,6 @@
       <c r="P378">
         <v>0.244</v>
       </c>
-      <c r="Q378">
-        <v>0</v>
-      </c>
-      <c r="R378">
-        <v>0</v>
-      </c>
-      <c r="S378">
-        <v>0</v>
-      </c>
       <c r="T378">
         <v>1.916</v>
       </c>
@@ -32512,15 +32128,6 @@
       <c r="P379">
         <v>1.018</v>
       </c>
-      <c r="Q379">
-        <v>0</v>
-      </c>
-      <c r="R379">
-        <v>0</v>
-      </c>
-      <c r="S379">
-        <v>0</v>
-      </c>
       <c r="T379">
         <v>2.739</v>
       </c>
@@ -32598,15 +32205,6 @@
       <c r="P380">
         <v>6.121</v>
       </c>
-      <c r="Q380">
-        <v>0</v>
-      </c>
-      <c r="R380">
-        <v>0</v>
-      </c>
-      <c r="S380">
-        <v>0</v>
-      </c>
       <c r="T380">
         <v>6.85</v>
       </c>
@@ -32684,15 +32282,6 @@
       <c r="P381">
         <v>0.8</v>
       </c>
-      <c r="Q381">
-        <v>0</v>
-      </c>
-      <c r="R381">
-        <v>0</v>
-      </c>
-      <c r="S381">
-        <v>0</v>
-      </c>
       <c r="T381">
         <v>11.475</v>
       </c>
@@ -32770,15 +32359,6 @@
       <c r="P382">
         <v>0.111</v>
       </c>
-      <c r="Q382">
-        <v>0</v>
-      </c>
-      <c r="R382">
-        <v>0</v>
-      </c>
-      <c r="S382">
-        <v>0</v>
-      </c>
       <c r="T382">
         <v>1.049</v>
       </c>
@@ -32942,15 +32522,6 @@
       <c r="P384">
         <v>7.067</v>
       </c>
-      <c r="Q384">
-        <v>0</v>
-      </c>
-      <c r="R384">
-        <v>0</v>
-      </c>
-      <c r="S384">
-        <v>0</v>
-      </c>
       <c r="T384">
         <v>1.638</v>
       </c>
@@ -33020,22 +32591,13 @@
         <v>1.27</v>
       </c>
       <c r="N385">
-        <v>68.52500000000001</v>
+        <v>68.524</v>
       </c>
       <c r="O385">
         <v>65.717</v>
       </c>
       <c r="P385">
         <v>4.467</v>
-      </c>
-      <c r="Q385">
-        <v>0</v>
-      </c>
-      <c r="R385">
-        <v>0</v>
-      </c>
-      <c r="S385">
-        <v>0</v>
       </c>
       <c r="T385">
         <v>0.307</v>
@@ -33106,22 +32668,13 @@
         <v>1.177</v>
       </c>
       <c r="N386">
-        <v>81.673</v>
+        <v>81.67400000000001</v>
       </c>
       <c r="O386">
         <v>65.136</v>
       </c>
       <c r="P386">
         <v>2.761</v>
-      </c>
-      <c r="Q386">
-        <v>0</v>
-      </c>
-      <c r="R386">
-        <v>0</v>
-      </c>
-      <c r="S386">
-        <v>0</v>
       </c>
       <c r="T386">
         <v>0.218</v>
@@ -33192,22 +32745,13 @@
         <v>0</v>
       </c>
       <c r="N387">
-        <v>56.579</v>
+        <v>56.57899999999999</v>
       </c>
       <c r="O387">
         <v>42.964</v>
       </c>
       <c r="P387">
         <v>13.59</v>
-      </c>
-      <c r="Q387">
-        <v>0</v>
-      </c>
-      <c r="R387">
-        <v>0</v>
-      </c>
-      <c r="S387">
-        <v>0</v>
       </c>
       <c r="T387">
         <v>22.655</v>
@@ -33278,22 +32822,13 @@
         <v>0.15</v>
       </c>
       <c r="N388">
-        <v>82.95399999999999</v>
+        <v>82.95400000000001</v>
       </c>
       <c r="O388">
         <v>69.91500000000001</v>
       </c>
       <c r="P388">
         <v>1.979</v>
-      </c>
-      <c r="Q388">
-        <v>0</v>
-      </c>
-      <c r="R388">
-        <v>0</v>
-      </c>
-      <c r="S388">
-        <v>0</v>
       </c>
       <c r="T388">
         <v>5.659</v>
@@ -33458,15 +32993,6 @@
       <c r="P390">
         <v>8.677</v>
       </c>
-      <c r="Q390">
-        <v>0</v>
-      </c>
-      <c r="R390">
-        <v>0</v>
-      </c>
-      <c r="S390">
-        <v>0</v>
-      </c>
       <c r="T390">
         <v>4.22</v>
       </c>
@@ -33802,15 +33328,6 @@
       <c r="P394">
         <v>1.65</v>
       </c>
-      <c r="Q394">
-        <v>0</v>
-      </c>
-      <c r="R394">
-        <v>0</v>
-      </c>
-      <c r="S394">
-        <v>0</v>
-      </c>
       <c r="T394">
         <v>1.465</v>
       </c>
@@ -34146,15 +33663,6 @@
       <c r="P398">
         <v>1.151</v>
       </c>
-      <c r="Q398">
-        <v>0</v>
-      </c>
-      <c r="R398">
-        <v>0</v>
-      </c>
-      <c r="S398">
-        <v>0</v>
-      </c>
       <c r="T398">
         <v>0</v>
       </c>
@@ -34232,15 +33740,6 @@
       <c r="P399">
         <v>0.369</v>
       </c>
-      <c r="Q399">
-        <v>0</v>
-      </c>
-      <c r="R399">
-        <v>0</v>
-      </c>
-      <c r="S399">
-        <v>0</v>
-      </c>
       <c r="T399">
         <v>3.105</v>
       </c>
@@ -34310,7 +33809,7 @@
         <v>0</v>
       </c>
       <c r="N400">
-        <v>84.80500000000001</v>
+        <v>84.804</v>
       </c>
       <c r="O400">
         <v>82.613</v>
@@ -34490,15 +33989,6 @@
       <c r="P402">
         <v>1.393</v>
       </c>
-      <c r="Q402">
-        <v>0</v>
-      </c>
-      <c r="R402">
-        <v>0</v>
-      </c>
-      <c r="S402">
-        <v>0</v>
-      </c>
       <c r="T402">
         <v>1.525</v>
       </c>
@@ -34568,22 +34058,13 @@
         <v>0</v>
       </c>
       <c r="N403">
-        <v>82.193</v>
+        <v>82.194</v>
       </c>
       <c r="O403">
         <v>76.527</v>
       </c>
       <c r="P403">
         <v>0.24</v>
-      </c>
-      <c r="Q403">
-        <v>0</v>
-      </c>
-      <c r="R403">
-        <v>0</v>
-      </c>
-      <c r="S403">
-        <v>0</v>
       </c>
       <c r="T403">
         <v>1.553</v>
@@ -34808,7 +34289,7 @@
         <v>0.103</v>
       </c>
       <c r="N406">
-        <v>84.24299999999999</v>
+        <v>84.24300000000001</v>
       </c>
       <c r="O406">
         <v>68.126</v>
@@ -34885,7 +34366,7 @@
         <v>0.097</v>
       </c>
       <c r="N407">
-        <v>83.907</v>
+        <v>83.90700000000001</v>
       </c>
       <c r="O407">
         <v>69.629</v>
@@ -34962,7 +34443,7 @@
         <v>1.16</v>
       </c>
       <c r="N408">
-        <v>84.34099999999999</v>
+        <v>84.34</v>
       </c>
       <c r="O408">
         <v>78.932</v>
@@ -35193,7 +34674,7 @@
         <v>0.004</v>
       </c>
       <c r="N411">
-        <v>74.70699999999999</v>
+        <v>74.708</v>
       </c>
       <c r="O411">
         <v>44.226</v>
@@ -35682,7 +35163,7 @@
         <v>7.866</v>
       </c>
       <c r="N417">
-        <v>69.18600000000001</v>
+        <v>69.185</v>
       </c>
       <c r="O417">
         <v>47.758</v>
@@ -35759,7 +35240,7 @@
         <v>0</v>
       </c>
       <c r="N418">
-        <v>72.66</v>
+        <v>72.661</v>
       </c>
       <c r="O418">
         <v>68.218</v>
@@ -35836,7 +35317,7 @@
         <v>3.088</v>
       </c>
       <c r="N419">
-        <v>80.468</v>
+        <v>80.467</v>
       </c>
       <c r="O419">
         <v>65.794</v>
@@ -36171,7 +35652,7 @@
         <v>1.003</v>
       </c>
       <c r="N423">
-        <v>77.718</v>
+        <v>77.71899999999999</v>
       </c>
       <c r="O423">
         <v>56.559</v>
@@ -36248,7 +35729,7 @@
         <v>0</v>
       </c>
       <c r="N424">
-        <v>75.78700000000001</v>
+        <v>75.78699999999999</v>
       </c>
       <c r="O424">
         <v>70.672</v>
@@ -36325,7 +35806,7 @@
         <v>0</v>
       </c>
       <c r="N425">
-        <v>80.56100000000001</v>
+        <v>80.56</v>
       </c>
       <c r="O425">
         <v>57.509</v>
@@ -36488,7 +35969,7 @@
         <v>0</v>
       </c>
       <c r="N427">
-        <v>81.601</v>
+        <v>81.60000000000001</v>
       </c>
       <c r="O427">
         <v>79.217</v>
@@ -36642,7 +36123,7 @@
         <v>0</v>
       </c>
       <c r="N429">
-        <v>83.358</v>
+        <v>83.357</v>
       </c>
       <c r="O429">
         <v>77.77</v>
@@ -36796,7 +36277,7 @@
         <v>0.395</v>
       </c>
       <c r="N431">
-        <v>89.276</v>
+        <v>89.27600000000001</v>
       </c>
       <c r="O431">
         <v>84.167</v>
@@ -36876,7 +36357,7 @@
         <v>0.34</v>
       </c>
       <c r="P432">
-        <v>11.61</v>
+        <v>11.611</v>
       </c>
       <c r="Q432">
         <v>0</v>
@@ -37436,7 +36917,7 @@
         <v>50.158</v>
       </c>
       <c r="P439">
-        <v>30.018</v>
+        <v>30.017</v>
       </c>
       <c r="Q439">
         <v>13.468</v>
@@ -37593,13 +37074,13 @@
         <v>0</v>
       </c>
       <c r="N441">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O441">
         <v>2</v>
       </c>
       <c r="P441">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="Q441">
         <v>0</v>
@@ -37679,13 +37160,13 @@
         <v>0</v>
       </c>
       <c r="N442">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="O442">
         <v>42</v>
       </c>
       <c r="P442">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="Q442">
         <v>0</v>
@@ -37773,15 +37254,6 @@
       <c r="P443">
         <v>20.4</v>
       </c>
-      <c r="Q443">
-        <v>0</v>
-      </c>
-      <c r="R443">
-        <v>0</v>
-      </c>
-      <c r="S443">
-        <v>0</v>
-      </c>
       <c r="T443">
         <v>0</v>
       </c>
@@ -37851,13 +37323,13 @@
         <v>0</v>
       </c>
       <c r="N444">
-        <v>0</v>
+        <v>38.7</v>
       </c>
       <c r="O444">
         <v>36</v>
       </c>
       <c r="P444">
-        <v>0</v>
+        <v>50.1</v>
       </c>
       <c r="Q444">
         <v>4</v>
@@ -37943,7 +37415,7 @@
         <v>0</v>
       </c>
       <c r="P445">
-        <v>0</v>
+        <v>87.90000000000001</v>
       </c>
       <c r="Q445">
         <v>9.5</v>
@@ -38029,7 +37501,7 @@
         <v>0</v>
       </c>
       <c r="P446">
-        <v>0</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="Q446">
         <v>0</v>
@@ -38109,13 +37581,13 @@
         <v>0</v>
       </c>
       <c r="N447">
-        <v>0</v>
+        <v>54.3</v>
       </c>
       <c r="O447">
         <v>53.8</v>
       </c>
       <c r="P447">
-        <v>0</v>
+        <v>33.7</v>
       </c>
       <c r="Q447">
         <v>12.7</v>
@@ -38201,7 +37673,7 @@
         <v>0</v>
       </c>
       <c r="P448">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q448">
         <v>20</v>
@@ -38287,7 +37759,7 @@
         <v>0</v>
       </c>
       <c r="P449">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="Q449">
         <v>85</v>
@@ -38373,7 +37845,7 @@
         <v>0</v>
       </c>
       <c r="P450">
-        <v>0</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="Q450">
         <v>84.3</v>
@@ -38459,7 +37931,7 @@
         <v>0</v>
       </c>
       <c r="P451">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q451">
         <v>10</v>
@@ -38539,13 +38011,13 @@
         <v>0</v>
       </c>
       <c r="N452">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O452">
         <v>15</v>
       </c>
       <c r="P452">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="Q452">
         <v>0</v>
@@ -38631,7 +38103,7 @@
         <v>0</v>
       </c>
       <c r="P453">
-        <v>0</v>
+        <v>49.3</v>
       </c>
       <c r="Q453">
         <v>34.5</v>
@@ -38711,13 +38183,13 @@
         <v>0</v>
       </c>
       <c r="N454">
-        <v>0</v>
+        <v>53.5</v>
       </c>
       <c r="O454">
         <v>53.3</v>
       </c>
       <c r="P454">
-        <v>0</v>
+        <v>40.4</v>
       </c>
       <c r="Q454">
         <v>0.8</v>
@@ -38797,13 +38269,13 @@
         <v>0</v>
       </c>
       <c r="N455">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="O455">
         <v>50</v>
       </c>
       <c r="P455">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="Q455">
         <v>10</v>
@@ -38883,13 +38355,13 @@
         <v>0</v>
       </c>
       <c r="N456">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O456">
         <v>0</v>
       </c>
       <c r="P456">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="Q456">
         <v>10</v>
@@ -38975,7 +38447,7 @@
         <v>0</v>
       </c>
       <c r="P457">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q457">
         <v>10</v>
@@ -39061,7 +38533,7 @@
         <v>0</v>
       </c>
       <c r="P458">
-        <v>0</v>
+        <v>95.8</v>
       </c>
       <c r="Q458">
         <v>40</v>
@@ -39141,13 +38613,13 @@
         <v>0</v>
       </c>
       <c r="N459">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O459">
         <v>10</v>
       </c>
       <c r="P459">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="Q459">
         <v>10</v>
@@ -39227,13 +38699,13 @@
         <v>0</v>
       </c>
       <c r="N460">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O460">
         <v>0</v>
       </c>
       <c r="P460">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="Q460">
         <v>98</v>
@@ -39319,7 +38791,7 @@
         <v>0</v>
       </c>
       <c r="P461">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="Q461">
         <v>30</v>
@@ -39405,7 +38877,7 @@
         <v>0</v>
       </c>
       <c r="P462">
-        <v>0</v>
+        <v>82.5</v>
       </c>
       <c r="Q462">
         <v>25</v>
@@ -39482,7 +38954,7 @@
         <v>0</v>
       </c>
       <c r="N463">
-        <v>99.995</v>
+        <v>99.994</v>
       </c>
       <c r="O463">
         <v>6.102</v>
@@ -40146,7 +39618,7 @@
         <v>0</v>
       </c>
       <c r="N471">
-        <v>99.038</v>
+        <v>99.03800000000001</v>
       </c>
       <c r="O471">
         <v>82.14400000000001</v>
@@ -40229,7 +39701,7 @@
         <v>0</v>
       </c>
       <c r="N472">
-        <v>52.138</v>
+        <v>52.13700000000001</v>
       </c>
       <c r="O472">
         <v>11.52</v>
@@ -40893,7 +40365,7 @@
         <v>0</v>
       </c>
       <c r="N480">
-        <v>82.383</v>
+        <v>82.38199999999999</v>
       </c>
       <c r="O480">
         <v>17.32</v>
@@ -41059,7 +40531,7 @@
         <v>0</v>
       </c>
       <c r="N482">
-        <v>93.988</v>
+        <v>93.989</v>
       </c>
       <c r="O482">
         <v>28.895</v>
@@ -41142,7 +40614,7 @@
         <v>0</v>
       </c>
       <c r="N483">
-        <v>80.413</v>
+        <v>80.41200000000001</v>
       </c>
       <c r="O483">
         <v>13.337</v>
@@ -41391,7 +40863,7 @@
         <v>0</v>
       </c>
       <c r="N486">
-        <v>91.465</v>
+        <v>91.464</v>
       </c>
       <c r="O486">
         <v>85.815</v>
@@ -41557,7 +41029,7 @@
         <v>0</v>
       </c>
       <c r="N488">
-        <v>80.773</v>
+        <v>80.77200000000001</v>
       </c>
       <c r="O488">
         <v>26.867</v>
@@ -41889,7 +41361,7 @@
         <v>0</v>
       </c>
       <c r="N492">
-        <v>75.31</v>
+        <v>75.30999999999999</v>
       </c>
       <c r="O492">
         <v>20.08</v>
@@ -42138,7 +41610,7 @@
         <v>0</v>
       </c>
       <c r="N495">
-        <v>71.042</v>
+        <v>71.041</v>
       </c>
       <c r="O495">
         <v>21.213</v>
@@ -42387,7 +41859,7 @@
         <v>0</v>
       </c>
       <c r="N498">
-        <v>56.028</v>
+        <v>56.029</v>
       </c>
       <c r="O498">
         <v>14.275</v>
@@ -42553,7 +42025,7 @@
         <v>0</v>
       </c>
       <c r="N500">
-        <v>63.719</v>
+        <v>63.71899999999999</v>
       </c>
       <c r="O500">
         <v>26.92</v>
@@ -42636,7 +42108,7 @@
         <v>0</v>
       </c>
       <c r="N501">
-        <v>42.799</v>
+        <v>42.8</v>
       </c>
       <c r="O501">
         <v>5.99</v>
@@ -42725,7 +42197,7 @@
         <v>23.9</v>
       </c>
       <c r="P502">
-        <v>2.677</v>
+        <v>2.676</v>
       </c>
       <c r="Q502">
         <v>0.006</v>
@@ -42802,7 +42274,7 @@
         <v>0</v>
       </c>
       <c r="N503">
-        <v>57.658</v>
+        <v>57.65799999999999</v>
       </c>
       <c r="O503">
         <v>15.385</v>
@@ -43134,7 +42606,7 @@
         <v>0</v>
       </c>
       <c r="N507">
-        <v>50.937</v>
+        <v>50.936</v>
       </c>
       <c r="O507">
         <v>10.972</v>
@@ -43217,7 +42689,7 @@
         <v>0</v>
       </c>
       <c r="N508">
-        <v>51.471</v>
+        <v>51.47</v>
       </c>
       <c r="O508">
         <v>0.336</v>
@@ -43300,7 +42772,7 @@
         <v>0</v>
       </c>
       <c r="N509">
-        <v>93.717</v>
+        <v>93.71599999999999</v>
       </c>
       <c r="O509">
         <v>77.937</v>
@@ -43466,7 +42938,7 @@
         <v>0</v>
       </c>
       <c r="N511">
-        <v>75.405</v>
+        <v>75.40600000000001</v>
       </c>
       <c r="O511">
         <v>18.099</v>
@@ -43549,7 +43021,7 @@
         <v>0</v>
       </c>
       <c r="N512">
-        <v>90.13</v>
+        <v>90.131</v>
       </c>
       <c r="O512">
         <v>10.615</v>
@@ -43715,7 +43187,7 @@
         <v>0</v>
       </c>
       <c r="N514">
-        <v>79.246</v>
+        <v>79.245</v>
       </c>
       <c r="O514">
         <v>5.291</v>
@@ -43964,7 +43436,7 @@
         <v>0</v>
       </c>
       <c r="N517">
-        <v>77.41200000000001</v>
+        <v>77.41300000000001</v>
       </c>
       <c r="O517">
         <v>20.602</v>
@@ -44379,7 +43851,7 @@
         <v>0</v>
       </c>
       <c r="N522">
-        <v>78.621</v>
+        <v>78.62100000000001</v>
       </c>
       <c r="O522">
         <v>29.655</v>
@@ -44462,7 +43934,7 @@
         <v>0</v>
       </c>
       <c r="N523">
-        <v>90.852</v>
+        <v>90.851</v>
       </c>
       <c r="O523">
         <v>3.376</v>
@@ -44711,7 +44183,7 @@
         <v>10.836</v>
       </c>
       <c r="N526">
-        <v>75.10299999999999</v>
+        <v>75.10300000000001</v>
       </c>
       <c r="O526">
         <v>47.469</v>
@@ -44877,7 +44349,7 @@
         <v>10.929</v>
       </c>
       <c r="N528">
-        <v>83.497</v>
+        <v>83.49799999999999</v>
       </c>
       <c r="O528">
         <v>77.705</v>
@@ -44960,7 +44432,7 @@
         <v>0</v>
       </c>
       <c r="N529">
-        <v>73.276</v>
+        <v>73.277</v>
       </c>
       <c r="O529">
         <v>58.621</v>
@@ -45043,7 +44515,7 @@
         <v>0</v>
       </c>
       <c r="N530">
-        <v>85.792</v>
+        <v>85.791</v>
       </c>
       <c r="O530">
         <v>6.688</v>
@@ -45292,7 +44764,7 @@
         <v>0</v>
       </c>
       <c r="N533">
-        <v>74.419</v>
+        <v>74.41900000000001</v>
       </c>
       <c r="O533">
         <v>41.279</v>
@@ -45375,13 +44847,13 @@
         <v>0</v>
       </c>
       <c r="N534">
-        <v>90.80800000000001</v>
+        <v>90.80799999999999</v>
       </c>
       <c r="O534">
         <v>41.64</v>
       </c>
       <c r="P534">
-        <v>1.624</v>
+        <v>1.625</v>
       </c>
       <c r="Q534">
         <v>0.436</v>
@@ -45458,7 +44930,7 @@
         <v>0</v>
       </c>
       <c r="N535">
-        <v>66.667</v>
+        <v>66.666</v>
       </c>
       <c r="O535">
         <v>20.974</v>
@@ -45541,13 +45013,13 @@
         <v>0.032</v>
       </c>
       <c r="N536">
-        <v>69.30200000000001</v>
+        <v>69.303</v>
       </c>
       <c r="O536">
         <v>36.098</v>
       </c>
       <c r="P536">
-        <v>3.519</v>
+        <v>3.518</v>
       </c>
       <c r="Q536">
         <v>0.227</v>
@@ -45624,13 +45096,13 @@
         <v>0</v>
       </c>
       <c r="N537">
-        <v>89.02200000000001</v>
+        <v>89.02199999999999</v>
       </c>
       <c r="O537">
         <v>21.136</v>
       </c>
       <c r="P537">
-        <v>1.956</v>
+        <v>1.955</v>
       </c>
       <c r="Q537">
         <v>0.946</v>

</xml_diff>